<commit_message>
remove sensitive data from report, update all buttons and pages
</commit_message>
<xml_diff>
--- a/features/support/Documents/Reference_List_Template.xlsx
+++ b/features/support/Documents/Reference_List_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngunida\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NewRubyFramework\btris_automation_regression_suite\features\support\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -847,7 +847,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,7 +866,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1746996</v>
+        <v>3635260</v>
       </c>
       <c r="B2" s="1">
         <v>36822</v>

</xml_diff>

<commit_message>
lab and radiology RL test
</commit_message>
<xml_diff>
--- a/features/support/Documents/Reference_List_Template.xlsx
+++ b/features/support/Documents/Reference_List_Template.xlsx
@@ -844,10 +844,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,7 +869,55 @@
         <v>3635260</v>
       </c>
       <c r="B2" s="1">
-        <v>36822</v>
+        <v>37399.552777777775</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3635260</v>
+      </c>
+      <c r="B3" s="1">
+        <v>37399.552777777775</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3635260</v>
+      </c>
+      <c r="B4" s="1">
+        <v>37399.552777777775</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3635260</v>
+      </c>
+      <c r="B5" s="1">
+        <v>37399.552777777775</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3635260</v>
+      </c>
+      <c r="B6" s="1">
+        <v>37399.552777777775</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3635260</v>
+      </c>
+      <c r="B7" s="1">
+        <v>37399.552777777775</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3635260</v>
+      </c>
+      <c r="B8" s="1">
+        <v>37399.552777777775</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding updates with Sandeep test branch
</commit_message>
<xml_diff>
--- a/features/support/Documents/Reference_List_Template.xlsx
+++ b/features/support/Documents/Reference_List_Template.xlsx
@@ -847,7 +847,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,50 +866,50 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3635260</v>
+        <v>7506405</v>
       </c>
       <c r="B2" s="1">
-        <v>37399.552777777775</v>
+        <v>42628</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3635260</v>
+        <v>9999997</v>
       </c>
       <c r="B3" s="1">
-        <v>37399.552777777775</v>
+        <v>39783</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3635260</v>
+        <v>3925535</v>
       </c>
       <c r="B4" s="1">
-        <v>37399.552777777775</v>
+        <v>40471</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3635260</v>
+        <v>4224188</v>
       </c>
       <c r="B5" s="1">
-        <v>37399.552777777775</v>
+        <v>40998</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3635260</v>
+        <v>1000007</v>
       </c>
       <c r="B6" s="1">
-        <v>37399.552777777775</v>
+        <v>42087</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3635260</v>
+        <v>2109372</v>
       </c>
       <c r="B7" s="1">
-        <v>37399.552777777775</v>
+        <v>40598</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updates to RL and more feature test
</commit_message>
<xml_diff>
--- a/features/support/Documents/Reference_List_Template.xlsx
+++ b/features/support/Documents/Reference_List_Template.xlsx
@@ -844,10 +844,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,58 +866,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>7506405</v>
+        <v>9999997</v>
       </c>
       <c r="B2" s="1">
-        <v>42628</v>
+        <v>39783</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>9999997</v>
+        <v>3925535</v>
       </c>
       <c r="B3" s="1">
-        <v>39783</v>
+        <v>40471</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3925535</v>
+        <v>4224188</v>
       </c>
       <c r="B4" s="1">
-        <v>40471</v>
+        <v>40998</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4224188</v>
+        <v>1000007</v>
       </c>
       <c r="B5" s="1">
-        <v>40998</v>
+        <v>42087</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1000007</v>
+        <v>2109372</v>
       </c>
       <c r="B6" s="1">
-        <v>42087</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2109372</v>
-      </c>
-      <c r="B7" s="1">
         <v>40598</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>3635260</v>
-      </c>
-      <c r="B8" s="1">
-        <v>37399.552777777775</v>
       </c>
     </row>
   </sheetData>

</xml_diff>